<commit_message>
Updated calibrations for 2 timesteps before exotic maturity
</commit_message>
<xml_diff>
--- a/nsde_2021_calibrations/Dynamic_calibration_hedging/Hedging_strategies.xlsx
+++ b/nsde_2021_calibrations/Dynamic_calibration_hedging/Hedging_strategies.xlsx
@@ -427,8 +427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:T32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="O22" sqref="O22:O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,14 +647,14 @@
         <v>16.190000000000001</v>
       </c>
       <c r="K7">
-        <f t="shared" ref="K7:K11" si="4">L7-L6</f>
+        <f t="shared" ref="K7:K10" si="4">L7-L6</f>
         <v>-0.12140000000000006</v>
       </c>
       <c r="L7">
         <v>-0.64990000000000003</v>
       </c>
       <c r="M7">
-        <f t="shared" ref="M7:M16" si="5">N7-N6</f>
+        <f t="shared" ref="M7:M15" si="5">N7-N6</f>
         <v>-4.1700000000000015E-2</v>
       </c>
       <c r="N7">
@@ -1092,7 +1092,7 @@
         <v>7.06</v>
       </c>
       <c r="K14">
-        <f t="shared" ref="K14:K16" si="24">L14-L13</f>
+        <f t="shared" ref="K14:K15" si="24">L14-L13</f>
         <v>-1.8600000000000061E-2</v>
       </c>
       <c r="L14">
@@ -1156,25 +1156,25 @@
       </c>
       <c r="K15">
         <f t="shared" si="24"/>
-        <v>-7.2500000000000009E-2</v>
+        <v>-1.0299999999999976E-2</v>
       </c>
       <c r="L15">
-        <v>-1.0622</v>
+        <v>-1</v>
       </c>
       <c r="M15">
         <f t="shared" si="5"/>
-        <v>1.430000000000009E-2</v>
+        <v>-0.12129999999999996</v>
       </c>
       <c r="N15">
-        <v>0.62770000000000004</v>
+        <v>0.49209999999999998</v>
       </c>
       <c r="O15">
         <f t="shared" si="25"/>
-        <v>857.84496296408895</v>
+        <v>806.24322096408889</v>
       </c>
       <c r="P15">
         <f t="shared" si="26"/>
-        <v>-494.86338039375721</v>
+        <v>-382.36826439375716</v>
       </c>
       <c r="Q15">
         <f t="shared" si="27"/>
@@ -1219,44 +1219,44 @@
       </c>
       <c r="K16">
         <f>L16-L15</f>
-        <v>1.0622</v>
+        <v>1</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
       <c r="M16">
         <f>N16-N15</f>
-        <v>-0.62770000000000004</v>
+        <v>-0.49209999999999998</v>
       </c>
       <c r="N16">
         <v>0</v>
       </c>
       <c r="O16" s="4">
         <f t="shared" si="25"/>
-        <v>-40.361299978082116</v>
+        <v>-39.366327194044743</v>
       </c>
       <c r="P16" s="3">
         <f t="shared" si="26"/>
-        <v>35.927269458750573</v>
+        <v>33.758164804161083</v>
       </c>
       <c r="Q16">
         <f t="shared" si="27"/>
-        <v>39.448700021917887</v>
+        <v>40.443672805955259</v>
       </c>
       <c r="R16">
         <f t="shared" si="28"/>
-        <v>35.927269458750573</v>
+        <v>33.758164804161083</v>
       </c>
       <c r="S16" s="2">
         <f t="shared" si="29"/>
-        <v>-7.5276605205863031E-2</v>
+        <v>-5.1953286311409851E-2</v>
       </c>
       <c r="T16" s="2">
         <f t="shared" si="30"/>
-        <v>0.22744343897337069</v>
-      </c>
-    </row>
-    <row r="17" spans="8:16" x14ac:dyDescent="0.25">
+        <v>0.1533366861688101</v>
+      </c>
+    </row>
+    <row r="17" spans="8:19" x14ac:dyDescent="0.25">
       <c r="O17" s="4" t="s">
         <v>19</v>
       </c>
@@ -1264,37 +1264,40 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="8:19" x14ac:dyDescent="0.25">
+      <c r="S21" s="2"/>
+    </row>
+    <row r="22" spans="8:19" x14ac:dyDescent="0.25">
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="8:19" x14ac:dyDescent="0.25">
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="8:19" x14ac:dyDescent="0.25">
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="8:19" x14ac:dyDescent="0.25">
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="8:19" x14ac:dyDescent="0.25">
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="8:19" x14ac:dyDescent="0.25">
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="8:19" x14ac:dyDescent="0.25">
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="8:19" x14ac:dyDescent="0.25">
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="8:19" x14ac:dyDescent="0.25">
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="8:19" x14ac:dyDescent="0.25">
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="8:19" x14ac:dyDescent="0.25">
       <c r="H32" s="1"/>
     </row>
   </sheetData>

</xml_diff>